<commit_message>
STEP file fixed, Gerbs Updated, BOM Finished
</commit_message>
<xml_diff>
--- a/Documentation/BOM.xlsx
+++ b/Documentation/BOM.xlsx
@@ -8,19 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\GitHub\DriveBoard_Hardware\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E29F54-03CF-4866-93D8-6B925DD7B5F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{013DF005-2065-451A-898E-9CFC34ED8C64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DriveBoard_2021" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="116">
   <si>
     <t>Id</t>
   </si>
@@ -55,18 +65,6 @@
     <t>TM4C129E_Launchpad</t>
   </si>
   <si>
-    <t>G***</t>
-  </si>
-  <si>
-    <t>0_MRDT_Logo_20mm</t>
-  </si>
-  <si>
-    <t>LOGO</t>
-  </si>
-  <si>
-    <t>z_sig_Jared_Allen</t>
-  </si>
-  <si>
     <t>Conn1</t>
   </si>
   <si>
@@ -121,9 +119,6 @@
     <t>LED4,LED9,LED10,LED11,LED12,LED13,LED17,LED18,LED19,LED20,LED21,LED22,LED23,LED24</t>
   </si>
   <si>
-    <t>pink</t>
-  </si>
-  <si>
     <t>LED5,LED6,LED7,LED8,LED14,LED15,LED16</t>
   </si>
   <si>
@@ -182,13 +177,214 @@
   </si>
   <si>
     <t>MCP2551-I-SN</t>
+  </si>
+  <si>
+    <t>Part Number</t>
+  </si>
+  <si>
+    <t>Vendor</t>
+  </si>
+  <si>
+    <t>Itrem Name</t>
+  </si>
+  <si>
+    <t>Cost Per Item</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>LAUNCHPAD TM4C129E EVAL BRD</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/texas-instruments/EK-TM4C129EXL/5764631</t>
+  </si>
+  <si>
+    <t>Digikey</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/rohm-semiconductor/ESR03EZPJ511/1762937</t>
+  </si>
+  <si>
+    <t>RHM510DCT-ND</t>
+  </si>
+  <si>
+    <t>RES SMD 510 OHM 5% 1/4W 0603</t>
+  </si>
+  <si>
+    <t>296-44249-ND</t>
+  </si>
+  <si>
+    <t>PCB Horizontal Bottom Contact</t>
+  </si>
+  <si>
+    <t>Red Housing</t>
+  </si>
+  <si>
+    <t>Black Housing</t>
+  </si>
+  <si>
+    <t>1336G1</t>
+  </si>
+  <si>
+    <t>Powerwerx</t>
+  </si>
+  <si>
+    <t>https://powerwerx.com/anderson-printed-circuit-board-pcb-contacts</t>
+  </si>
+  <si>
+    <t>https://powerwerx.com/anderson-powerpole-colored-housings</t>
+  </si>
+  <si>
+    <t>Violet Housing</t>
+  </si>
+  <si>
+    <t>1327G6</t>
+  </si>
+  <si>
+    <t>1327G23</t>
+  </si>
+  <si>
+    <t>Conn3,Conn1</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/molex/0705530002/114955?s=N4IgTCBcDaIOoFkAsBOADARgLQDkAiIAugL5A</t>
+  </si>
+  <si>
+    <t>WM4901-ND</t>
+  </si>
+  <si>
+    <t>Yellow Housing</t>
+  </si>
+  <si>
+    <t>1327G16</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/molex/0705530001/114951?s=N4IgTCBcDaIOoFkAsBOADGgtAOQCIgF0BfIA</t>
+  </si>
+  <si>
+    <t>WM4900-ND</t>
+  </si>
+  <si>
+    <t>CONN HEADER R/A 2POS 2.54MM</t>
+  </si>
+  <si>
+    <t>CONN HEADER R/A 3POS 2.54MM</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL10B106MQ8NRNC/3887606?s=N4IgTCBcDaIDoBcDCAZAjABgEKYGwFkBFADgDkAlUpEAXQF8g</t>
+  </si>
+  <si>
+    <t>CL10B106MQ8NRNC</t>
+  </si>
+  <si>
+    <t>CAP CER 10UF 6.3V X7R 0603</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/lite-on-inc/LTST-C191KGKT/386834</t>
+  </si>
+  <si>
+    <t>LED GREEN CLEAR SMD</t>
+  </si>
+  <si>
+    <t>LTST-C191KGKT</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/lite-on-inc/LTST-C191KSKT/386838</t>
+  </si>
+  <si>
+    <t>LED YELLOW CLEAR SMD</t>
+  </si>
+  <si>
+    <t>LTST-C191KSKT</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/lite-on-inc/LTST-C191TBKT/573587</t>
+  </si>
+  <si>
+    <t>LED BLUE CLEAR CHIP SMD</t>
+  </si>
+  <si>
+    <t>LTST-C191TBKT</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/rohm-semiconductor/ESR03EZPJ102/1762924</t>
+  </si>
+  <si>
+    <t>ESR03EZPJ102</t>
+  </si>
+  <si>
+    <t>RES SMD 1K OHM 5% 1/4W 0603</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/rohm-semiconductor/ESR03EZPJ331/1762730</t>
+  </si>
+  <si>
+    <t>ESR03EZPJ331</t>
+  </si>
+  <si>
+    <t>RES SMD 330 OHM 5% 1/4W 0603</t>
+  </si>
+  <si>
+    <t>RES SMD 120 OHM 5% 1/4W 0603ESR03EZPJ121</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/rohm-semiconductor/ESR03EZPJ121/1983454</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/e-switch/TL3305AF160QG/5816195</t>
+  </si>
+  <si>
+    <t>SWITCH TACTILE SPST-NO 50MA 12V</t>
+  </si>
+  <si>
+    <t>TL3305AF160QG</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/c-k/OS102011MA1QN1/1981430?s=N4IgTCBcDaIMIGkByBOArGlBaJAREAugL5A</t>
+  </si>
+  <si>
+    <t>SWITCH SLIDE SPDT 100MA 12V</t>
+  </si>
+  <si>
+    <t>OS102011MA1QN1</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/murata-power-solutions-inc/OKI-78SR-5-1.5-W36H-C/3438675</t>
+  </si>
+  <si>
+    <t>DC DC CONVERTER 5V 8W</t>
+  </si>
+  <si>
+    <t>OKI-78SR-5/1.5-W36H-Chttps://www.digikey.com/en/products/detail/murata-power-solutions-inc/OKI-78SR-3.3-1.5-W36H-C/4878851</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/murata-power-solutions-inc/OKI-78SR-3.3-1.5-W36H-C/4878851</t>
+  </si>
+  <si>
+    <t>DC DC CONVERTER 3.3V 5W</t>
+  </si>
+  <si>
+    <t>OKI-78SR-3.3/1.5-W36H-C</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/microchip-technology/mcp2551-i-sn/509452</t>
+  </si>
+  <si>
+    <t>IC TRANSCEIVER HALF 1/1 8SOIC</t>
+  </si>
+  <si>
+    <t>MCP2551-I/SN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -323,6 +519,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -621,7 +831,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -664,11 +874,17 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -702,6 +918,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1022,19 +1239,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="81.85546875" customWidth="1"/>
-    <col min="3" max="3" width="50.28515625" customWidth="1"/>
-    <col min="5" max="5" width="23.42578125" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
+    <col min="3" max="3" width="44.7109375" customWidth="1"/>
+    <col min="4" max="5" width="23.42578125" customWidth="1"/>
+    <col min="6" max="6" width="23.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" customWidth="1"/>
+    <col min="10" max="10" width="8.7109375" customWidth="1"/>
+    <col min="11" max="11" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1045,16 +1268,31 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1064,14 +1302,32 @@
       <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
+        <v>500</v>
+      </c>
+      <c r="E2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H2">
         <v>15</v>
       </c>
-      <c r="E2">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <v>0.1</v>
+      </c>
+      <c r="J2" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="K2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1081,14 +1337,32 @@
       <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H3">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <v>29.99</v>
+      </c>
+      <c r="J3">
+        <v>29.99</v>
+      </c>
+      <c r="K3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1098,14 +1372,32 @@
       <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="D4">
-        <v>1</v>
+      <c r="D4" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="F4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G4" t="s">
+        <v>65</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4">
+        <v>0.59</v>
+      </c>
+      <c r="J4">
+        <v>1.77</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1113,288 +1405,712 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1327</v>
+      </c>
+      <c r="G5" t="s">
+        <v>65</v>
+      </c>
+      <c r="H5">
         <v>1</v>
       </c>
-      <c r="E5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <v>0.37</v>
+      </c>
+      <c r="J5">
+        <v>0.37</v>
+      </c>
+      <c r="K5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6">
+        <v>12</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" t="s">
+        <v>69</v>
+      </c>
+      <c r="G6" t="s">
+        <v>65</v>
+      </c>
+      <c r="H6">
         <v>1</v>
       </c>
-      <c r="E6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <v>0.37</v>
+      </c>
+      <c r="J6">
+        <v>0.37</v>
+      </c>
+      <c r="K6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="F7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G7" t="s">
+        <v>65</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>0.39</v>
+      </c>
+      <c r="J7">
+        <v>0.39</v>
+      </c>
+      <c r="K7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
-      <c r="E8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F8" t="s">
+        <v>73</v>
+      </c>
+      <c r="G8" t="s">
+        <v>56</v>
+      </c>
+      <c r="H8">
+        <v>10</v>
+      </c>
+      <c r="I8">
+        <v>0.72799999999999998</v>
+      </c>
+      <c r="J8">
+        <v>7.28</v>
+      </c>
+      <c r="K8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9">
-        <v>2</v>
+        <v>18</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="E9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="F9" t="s">
+        <v>64</v>
+      </c>
+      <c r="G9" t="s">
+        <v>65</v>
+      </c>
+      <c r="H9">
+        <v>4</v>
+      </c>
+      <c r="I9">
+        <v>0.59</v>
+      </c>
+      <c r="J9">
+        <v>1.18</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>71</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10">
-        <v>6</v>
+        <v>18</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="E10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1327</v>
+      </c>
+      <c r="G10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H10">
+        <v>2</v>
+      </c>
+      <c r="I10">
+        <v>0.37</v>
+      </c>
+      <c r="J10">
+        <v>0.74</v>
+      </c>
+      <c r="K10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11">
-        <v>4</v>
+        <v>18</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="E11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="F11" t="s">
+        <v>75</v>
+      </c>
+      <c r="G11" t="s">
+        <v>65</v>
+      </c>
+      <c r="H11">
+        <v>2</v>
+      </c>
+      <c r="I11">
+        <v>0.39</v>
+      </c>
+      <c r="J11">
+        <v>0.78</v>
+      </c>
+      <c r="K11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12">
-        <v>14</v>
+        <v>20</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="E12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="F12" t="s">
+        <v>77</v>
+      </c>
+      <c r="G12" t="s">
+        <v>56</v>
+      </c>
+      <c r="H12">
+        <v>2</v>
+      </c>
+      <c r="I12">
+        <v>0.74</v>
+      </c>
+      <c r="J12">
+        <v>1.48</v>
+      </c>
+      <c r="K12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13">
-        <v>7</v>
+        <v>23</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="E13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+      <c r="F13" t="s">
+        <v>81</v>
+      </c>
+      <c r="G13" t="s">
+        <v>56</v>
+      </c>
+      <c r="H13">
+        <v>6</v>
+      </c>
+      <c r="I13">
+        <v>0.78</v>
+      </c>
+      <c r="J13">
+        <v>4.68</v>
+      </c>
+      <c r="K13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14">
-        <v>2</v>
+        <v>26</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="E14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+      <c r="F14" t="s">
+        <v>85</v>
+      </c>
+      <c r="G14" t="s">
+        <v>56</v>
+      </c>
+      <c r="H14">
+        <v>4</v>
+      </c>
+      <c r="I14">
+        <v>0.26</v>
+      </c>
+      <c r="J14">
+        <v>1.04</v>
+      </c>
+      <c r="K14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="C15" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15">
-        <v>8</v>
-      </c>
-      <c r="E15">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" t="s">
+        <v>88</v>
+      </c>
+      <c r="F15" t="s">
+        <v>89</v>
+      </c>
+      <c r="G15" t="s">
+        <v>56</v>
+      </c>
+      <c r="H15">
+        <v>14</v>
+      </c>
+      <c r="I15">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="J15">
+        <f>I15*H15</f>
+        <v>3.9200000000000004</v>
+      </c>
+      <c r="K15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="C16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E16" t="s">
+        <v>91</v>
+      </c>
+      <c r="F16" t="s">
+        <v>92</v>
+      </c>
+      <c r="G16" t="s">
+        <v>56</v>
+      </c>
+      <c r="H16">
         <v>7</v>
       </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <v>0.33</v>
+      </c>
+      <c r="J16">
+        <f t="shared" ref="J16:J24" si="0">I16*H16</f>
+        <v>2.31</v>
+      </c>
+      <c r="K16" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C17" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="E17" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="F17" t="s">
+        <v>94</v>
+      </c>
+      <c r="G17" t="s">
+        <v>56</v>
+      </c>
+      <c r="H17">
+        <v>2</v>
+      </c>
+      <c r="I17">
+        <v>0.1</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="K17" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C18" t="s">
-        <v>44</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="D18" s="1">
+        <v>330</v>
       </c>
       <c r="E18" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="F18" t="s">
+        <v>97</v>
+      </c>
+      <c r="G18" t="s">
+        <v>56</v>
+      </c>
+      <c r="H18">
+        <v>8</v>
+      </c>
+      <c r="I18">
+        <v>0.1</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+      <c r="K18" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="C19" t="s">
-        <v>47</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="D19" s="1">
+        <v>120</v>
       </c>
       <c r="E19" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="G19" t="s">
+        <v>56</v>
+      </c>
+      <c r="H19">
+        <v>5</v>
+      </c>
+      <c r="I19">
+        <v>0.1</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="K19" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="C20" t="s">
-        <v>47</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
+        <v>36</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="E20" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="F20" t="s">
+        <v>103</v>
+      </c>
+      <c r="G20" t="s">
+        <v>56</v>
+      </c>
+      <c r="H20">
+        <v>6</v>
+      </c>
+      <c r="I20">
+        <v>0.18</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="0"/>
+        <v>1.08</v>
+      </c>
+      <c r="K20" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="C21" t="s">
-        <v>52</v>
-      </c>
-      <c r="D21">
+        <v>39</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" t="s">
+        <v>105</v>
+      </c>
+      <c r="F21" t="s">
+        <v>106</v>
+      </c>
+      <c r="G21" t="s">
+        <v>56</v>
+      </c>
+      <c r="H21">
         <v>1</v>
       </c>
-      <c r="E21" t="s">
-        <v>53</v>
+      <c r="I21">
+        <v>0.48</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="0"/>
+        <v>0.48</v>
+      </c>
+      <c r="K21" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" t="s">
+        <v>111</v>
+      </c>
+      <c r="F22" t="s">
+        <v>112</v>
+      </c>
+      <c r="G22" t="s">
+        <v>56</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>4.3</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="0"/>
+        <v>4.3</v>
+      </c>
+      <c r="K22" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E23" t="s">
+        <v>108</v>
+      </c>
+      <c r="F23" t="s">
+        <v>109</v>
+      </c>
+      <c r="G23" t="s">
+        <v>56</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>4.3</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="0"/>
+        <v>4.3</v>
+      </c>
+      <c r="K23" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E24" t="s">
+        <v>114</v>
+      </c>
+      <c r="F24" t="s">
+        <v>115</v>
+      </c>
+      <c r="G24" t="s">
+        <v>56</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <v>1.02</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="0"/>
+        <v>1.02</v>
+      </c>
+      <c r="K24" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="K4" r:id="rId1" xr:uid="{D2357DE8-65CA-4770-A76E-B2B579E41297}"/>
+    <hyperlink ref="K9" r:id="rId2" xr:uid="{5C0C9641-F89C-429D-9BDA-83A8AA52671E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Digikey Part Number
</commit_message>
<xml_diff>
--- a/Documentation/BOM.xlsx
+++ b/Documentation/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\GitHub\DriveBoard_Hardware\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{013DF005-2065-451A-898E-9CFC34ED8C64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D516CD3F-9988-4C4F-8F1B-B02B2029EA35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="132">
   <si>
     <t>Id</t>
   </si>
@@ -179,9 +179,6 @@
     <t>MCP2551-I-SN</t>
   </si>
   <si>
-    <t>Part Number</t>
-  </si>
-  <si>
     <t>Vendor</t>
   </si>
   <si>
@@ -194,12 +191,6 @@
     <t>Cost</t>
   </si>
   <si>
-    <t>LAUNCHPAD TM4C129E EVAL BRD</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/texas-instruments/EK-TM4C129EXL/5764631</t>
-  </si>
-  <si>
     <t>Digikey</t>
   </si>
   <si>
@@ -212,9 +203,6 @@
     <t>RES SMD 510 OHM 5% 1/4W 0603</t>
   </si>
   <si>
-    <t>296-44249-ND</t>
-  </si>
-  <si>
     <t>PCB Horizontal Bottom Contact</t>
   </si>
   <si>
@@ -359,9 +347,6 @@
     <t>DC DC CONVERTER 5V 8W</t>
   </si>
   <si>
-    <t>OKI-78SR-5/1.5-W36H-Chttps://www.digikey.com/en/products/detail/murata-power-solutions-inc/OKI-78SR-3.3-1.5-W36H-C/4878851</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/en/products/detail/murata-power-solutions-inc/OKI-78SR-3.3-1.5-W36H-C/4878851</t>
   </si>
   <si>
@@ -378,6 +363,69 @@
   </si>
   <si>
     <t>MCP2551-I/SN</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/texas-instruments/EK-TM4C1294XL/4725808</t>
+  </si>
+  <si>
+    <t>Manufacture Part Number</t>
+  </si>
+  <si>
+    <t>OKI-78SR-5/1.5-W36H-C</t>
+  </si>
+  <si>
+    <t>296-37267-ND</t>
+  </si>
+  <si>
+    <t>EK-TM4C1294XL</t>
+  </si>
+  <si>
+    <t>ESR03EZPJ511</t>
+  </si>
+  <si>
+    <t>LAUNCHPAD TM4C129X EVAL BRD</t>
+  </si>
+  <si>
+    <t>Vendor Part Number</t>
+  </si>
+  <si>
+    <t>1276-1948-1-ND</t>
+  </si>
+  <si>
+    <t>160-1446-1-ND</t>
+  </si>
+  <si>
+    <t>160-1448-1-ND</t>
+  </si>
+  <si>
+    <t>160-1647-1-ND</t>
+  </si>
+  <si>
+    <t>RHM1.0KDCT-ND</t>
+  </si>
+  <si>
+    <t>RHM330DCT-ND</t>
+  </si>
+  <si>
+    <t>RHM120DCT-ND</t>
+  </si>
+  <si>
+    <t>ESR03EZPJ121</t>
+  </si>
+  <si>
+    <t>EG5350CT-ND</t>
+  </si>
+  <si>
+    <t>CKN9559-ND</t>
+  </si>
+  <si>
+    <t>811-3014-ND</t>
+  </si>
+  <si>
+    <t>811-2692-ND</t>
+  </si>
+  <si>
+    <t>MCP2551-I/SN-ND</t>
   </si>
 </sst>
 </file>
@@ -1239,25 +1287,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19.42578125" customWidth="1"/>
     <col min="3" max="3" width="44.7109375" customWidth="1"/>
-    <col min="4" max="5" width="23.42578125" customWidth="1"/>
-    <col min="6" max="6" width="23.7109375" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" customWidth="1"/>
-    <col min="10" max="10" width="8.7109375" customWidth="1"/>
-    <col min="11" max="11" width="19.140625" customWidth="1"/>
+    <col min="4" max="6" width="23.42578125" customWidth="1"/>
+    <col min="7" max="7" width="24.85546875" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" customWidth="1"/>
+    <col min="11" max="11" width="8.7109375" customWidth="1"/>
+    <col min="12" max="12" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1271,28 +1319,31 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" t="s">
         <v>51</v>
       </c>
-      <c r="F1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>52</v>
       </c>
-      <c r="J1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1306,28 +1357,31 @@
         <v>500</v>
       </c>
       <c r="E2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G2" t="s">
-        <v>56</v>
-      </c>
-      <c r="H2">
+        <v>116</v>
+      </c>
+      <c r="H2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2">
         <v>15</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>0.1</v>
       </c>
-      <c r="J2" s="2">
+      <c r="K2" s="2">
         <v>1.5</v>
       </c>
-      <c r="K2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1341,28 +1395,31 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>54</v>
+        <v>117</v>
       </c>
       <c r="F3" t="s">
-        <v>60</v>
+        <v>114</v>
       </c>
       <c r="G3" t="s">
-        <v>56</v>
-      </c>
-      <c r="H3">
+        <v>115</v>
+      </c>
+      <c r="H3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I3">
         <v>1</v>
       </c>
-      <c r="I3">
-        <v>29.99</v>
-      </c>
       <c r="J3">
-        <v>29.99</v>
-      </c>
-      <c r="K3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <v>23.99</v>
+      </c>
+      <c r="K3">
+        <v>23.99</v>
+      </c>
+      <c r="L3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1376,28 +1433,31 @@
         <v>13</v>
       </c>
       <c r="E4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4" t="s">
+        <v>60</v>
+      </c>
+      <c r="H4" t="s">
         <v>61</v>
       </c>
-      <c r="F4" t="s">
-        <v>64</v>
-      </c>
-      <c r="G4" t="s">
-        <v>65</v>
-      </c>
-      <c r="H4">
+      <c r="I4">
         <v>3</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>0.59</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>1.77</v>
       </c>
-      <c r="K4" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1411,28 +1471,31 @@
         <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F5" s="1">
         <v>1327</v>
       </c>
-      <c r="G5" t="s">
-        <v>65</v>
-      </c>
-      <c r="H5">
+      <c r="G5" s="1">
+        <v>1327</v>
+      </c>
+      <c r="H5" t="s">
+        <v>61</v>
+      </c>
+      <c r="I5">
         <v>1</v>
-      </c>
-      <c r="I5">
-        <v>0.37</v>
       </c>
       <c r="J5">
         <v>0.37</v>
       </c>
-      <c r="K5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K5">
+        <v>0.37</v>
+      </c>
+      <c r="L5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1446,28 +1509,31 @@
         <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F6" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G6" t="s">
         <v>65</v>
       </c>
-      <c r="H6">
+      <c r="H6" t="s">
+        <v>61</v>
+      </c>
+      <c r="I6">
         <v>1</v>
-      </c>
-      <c r="I6">
-        <v>0.37</v>
       </c>
       <c r="J6">
         <v>0.37</v>
       </c>
-      <c r="K6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K6">
+        <v>0.37</v>
+      </c>
+      <c r="L6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1481,28 +1547,31 @@
         <v>13</v>
       </c>
       <c r="E7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G7" t="s">
-        <v>65</v>
-      </c>
-      <c r="H7">
+        <v>66</v>
+      </c>
+      <c r="H7" t="s">
+        <v>61</v>
+      </c>
+      <c r="I7">
         <v>1</v>
-      </c>
-      <c r="I7">
-        <v>0.39</v>
       </c>
       <c r="J7">
         <v>0.39</v>
       </c>
-      <c r="K7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K7">
+        <v>0.39</v>
+      </c>
+      <c r="L7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1516,33 +1585,36 @@
         <v>16</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F8" t="s">
-        <v>73</v>
-      </c>
-      <c r="G8" t="s">
-        <v>56</v>
-      </c>
-      <c r="H8">
+        <v>75</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G8" s="1">
+        <v>705530002</v>
+      </c>
+      <c r="H8" t="s">
+        <v>53</v>
+      </c>
+      <c r="I8">
         <v>10</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>0.72799999999999998</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>7.28</v>
       </c>
-      <c r="K8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C9" t="s">
         <v>18</v>
@@ -1551,33 +1623,36 @@
         <v>13</v>
       </c>
       <c r="E9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" t="s">
+        <v>60</v>
+      </c>
+      <c r="G9" t="s">
+        <v>60</v>
+      </c>
+      <c r="H9" t="s">
         <v>61</v>
       </c>
-      <c r="F9" t="s">
-        <v>64</v>
-      </c>
-      <c r="G9" t="s">
-        <v>65</v>
-      </c>
-      <c r="H9">
+      <c r="I9">
         <v>4</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>0.59</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>1.18</v>
       </c>
-      <c r="K9" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C10" t="s">
         <v>18</v>
@@ -1586,28 +1661,31 @@
         <v>13</v>
       </c>
       <c r="E10" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F10" s="1">
         <v>1327</v>
       </c>
-      <c r="G10" t="s">
-        <v>65</v>
-      </c>
-      <c r="H10">
+      <c r="G10" s="1">
+        <v>1327</v>
+      </c>
+      <c r="H10" t="s">
+        <v>61</v>
+      </c>
+      <c r="I10">
         <v>2</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>0.37</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>0.74</v>
       </c>
-      <c r="K10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1621,28 +1699,31 @@
         <v>13</v>
       </c>
       <c r="E11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F11" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G11" t="s">
-        <v>65</v>
-      </c>
-      <c r="H11">
+        <v>71</v>
+      </c>
+      <c r="H11" t="s">
+        <v>61</v>
+      </c>
+      <c r="I11">
         <v>2</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>0.39</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>0.78</v>
       </c>
-      <c r="K11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1656,28 +1737,31 @@
         <v>21</v>
       </c>
       <c r="E12" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F12" t="s">
-        <v>77</v>
-      </c>
-      <c r="G12" t="s">
-        <v>56</v>
-      </c>
-      <c r="H12">
+        <v>73</v>
+      </c>
+      <c r="G12" s="1">
+        <v>705530001</v>
+      </c>
+      <c r="H12" t="s">
+        <v>53</v>
+      </c>
+      <c r="I12">
         <v>2</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>0.74</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>1.48</v>
       </c>
-      <c r="K12" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1691,28 +1775,31 @@
         <v>24</v>
       </c>
       <c r="E13" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F13" t="s">
-        <v>81</v>
+        <v>119</v>
       </c>
       <c r="G13" t="s">
-        <v>56</v>
-      </c>
-      <c r="H13">
+        <v>77</v>
+      </c>
+      <c r="H13" t="s">
+        <v>53</v>
+      </c>
+      <c r="I13">
         <v>6</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>0.78</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>4.68</v>
       </c>
-      <c r="K13" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1726,28 +1813,31 @@
         <v>27</v>
       </c>
       <c r="E14" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F14" t="s">
-        <v>85</v>
+        <v>120</v>
       </c>
       <c r="G14" t="s">
-        <v>56</v>
-      </c>
-      <c r="H14">
+        <v>81</v>
+      </c>
+      <c r="H14" t="s">
+        <v>53</v>
+      </c>
+      <c r="I14">
         <v>4</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>0.26</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>1.04</v>
       </c>
-      <c r="K14" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1761,29 +1851,32 @@
         <v>30</v>
       </c>
       <c r="E15" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F15" t="s">
-        <v>89</v>
+        <v>121</v>
       </c>
       <c r="G15" t="s">
-        <v>56</v>
-      </c>
-      <c r="H15">
+        <v>85</v>
+      </c>
+      <c r="H15" t="s">
+        <v>53</v>
+      </c>
+      <c r="I15">
         <v>14</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>0.28000000000000003</v>
       </c>
-      <c r="J15">
-        <f>I15*H15</f>
+      <c r="K15">
+        <f>J15*I15</f>
         <v>3.9200000000000004</v>
       </c>
-      <c r="K15" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1794,32 +1887,35 @@
         <v>26</v>
       </c>
       <c r="D16" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E16" t="s">
+        <v>87</v>
+      </c>
+      <c r="F16" t="s">
+        <v>122</v>
+      </c>
+      <c r="G16" t="s">
+        <v>88</v>
+      </c>
+      <c r="H16" t="s">
+        <v>53</v>
+      </c>
+      <c r="I16">
+        <v>7</v>
+      </c>
+      <c r="J16">
+        <v>0.33</v>
+      </c>
+      <c r="K16">
+        <f t="shared" ref="K16:K24" si="0">J16*I16</f>
+        <v>2.31</v>
+      </c>
+      <c r="L16" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="E16" t="s">
-        <v>91</v>
-      </c>
-      <c r="F16" t="s">
-        <v>92</v>
-      </c>
-      <c r="G16" t="s">
-        <v>56</v>
-      </c>
-      <c r="H16">
-        <v>7</v>
-      </c>
-      <c r="I16">
-        <v>0.33</v>
-      </c>
-      <c r="J16">
-        <f t="shared" ref="J16:J24" si="0">I16*H16</f>
-        <v>2.31</v>
-      </c>
-      <c r="K16" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1833,29 +1929,32 @@
         <v>32</v>
       </c>
       <c r="E17" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F17" t="s">
-        <v>94</v>
+        <v>123</v>
       </c>
       <c r="G17" t="s">
-        <v>56</v>
-      </c>
-      <c r="H17">
+        <v>90</v>
+      </c>
+      <c r="H17" t="s">
+        <v>53</v>
+      </c>
+      <c r="I17">
         <v>2</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>0.1</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="K17" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1869,29 +1968,32 @@
         <v>330</v>
       </c>
       <c r="E18" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F18" t="s">
-        <v>97</v>
+        <v>124</v>
       </c>
       <c r="G18" t="s">
-        <v>56</v>
-      </c>
-      <c r="H18">
+        <v>93</v>
+      </c>
+      <c r="H18" t="s">
+        <v>53</v>
+      </c>
+      <c r="I18">
         <v>8</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>0.1</v>
       </c>
-      <c r="J18">
+      <c r="K18">
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
-      <c r="K18" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L18" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1905,26 +2007,32 @@
         <v>120</v>
       </c>
       <c r="E19" t="s">
-        <v>99</v>
+        <v>95</v>
+      </c>
+      <c r="F19" t="s">
+        <v>125</v>
       </c>
       <c r="G19" t="s">
-        <v>56</v>
-      </c>
-      <c r="H19">
+        <v>126</v>
+      </c>
+      <c r="H19" t="s">
+        <v>53</v>
+      </c>
+      <c r="I19">
         <v>5</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <v>0.1</v>
       </c>
-      <c r="J19">
+      <c r="K19">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="K19" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1938,29 +2046,32 @@
         <v>37</v>
       </c>
       <c r="E20" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F20" t="s">
-        <v>103</v>
+        <v>127</v>
       </c>
       <c r="G20" t="s">
-        <v>56</v>
-      </c>
-      <c r="H20">
+        <v>99</v>
+      </c>
+      <c r="H20" t="s">
+        <v>53</v>
+      </c>
+      <c r="I20">
         <v>6</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <v>0.18</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <f t="shared" si="0"/>
         <v>1.08</v>
       </c>
-      <c r="K20" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L20" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1974,29 +2085,32 @@
         <v>40</v>
       </c>
       <c r="E21" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F21" t="s">
-        <v>106</v>
+        <v>128</v>
       </c>
       <c r="G21" t="s">
-        <v>56</v>
-      </c>
-      <c r="H21">
+        <v>102</v>
+      </c>
+      <c r="H21" t="s">
+        <v>53</v>
+      </c>
+      <c r="I21">
         <v>1</v>
       </c>
-      <c r="I21">
+      <c r="J21">
         <v>0.48</v>
       </c>
-      <c r="J21">
+      <c r="K21">
         <f t="shared" si="0"/>
         <v>0.48</v>
       </c>
-      <c r="K21" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L21" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2010,29 +2124,32 @@
         <v>43</v>
       </c>
       <c r="E22" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="F22" t="s">
-        <v>112</v>
+        <v>129</v>
       </c>
       <c r="G22" t="s">
-        <v>56</v>
-      </c>
-      <c r="H22">
+        <v>107</v>
+      </c>
+      <c r="H22" t="s">
+        <v>53</v>
+      </c>
+      <c r="I22">
         <v>1</v>
       </c>
-      <c r="I22">
+      <c r="J22">
         <v>4.3</v>
       </c>
-      <c r="J22">
+      <c r="K22">
         <f t="shared" si="0"/>
         <v>4.3</v>
       </c>
-      <c r="K22" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L22" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2046,29 +2163,32 @@
         <v>45</v>
       </c>
       <c r="E23" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="F23" t="s">
-        <v>109</v>
+        <v>130</v>
       </c>
       <c r="G23" t="s">
-        <v>56</v>
-      </c>
-      <c r="H23">
+        <v>113</v>
+      </c>
+      <c r="H23" t="s">
+        <v>53</v>
+      </c>
+      <c r="I23">
         <v>1</v>
       </c>
-      <c r="I23">
+      <c r="J23">
         <v>4.3</v>
       </c>
-      <c r="J23">
+      <c r="K23">
         <f t="shared" si="0"/>
         <v>4.3</v>
       </c>
-      <c r="K23" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L23" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2082,35 +2202,42 @@
         <v>48</v>
       </c>
       <c r="E24" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="F24" t="s">
-        <v>115</v>
+        <v>131</v>
       </c>
       <c r="G24" t="s">
-        <v>56</v>
-      </c>
-      <c r="H24">
+        <v>110</v>
+      </c>
+      <c r="H24" t="s">
+        <v>53</v>
+      </c>
+      <c r="I24">
         <v>1</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <v>1.02</v>
       </c>
-      <c r="J24">
+      <c r="K24">
         <f t="shared" si="0"/>
         <v>1.02</v>
       </c>
-      <c r="K24" t="s">
-        <v>113</v>
+      <c r="L24" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="K4" r:id="rId1" xr:uid="{D2357DE8-65CA-4770-A76E-B2B579E41297}"/>
-    <hyperlink ref="K9" r:id="rId2" xr:uid="{5C0C9641-F89C-429D-9BDA-83A8AA52671E}"/>
+    <hyperlink ref="L4" r:id="rId1" xr:uid="{D2357DE8-65CA-4770-A76E-B2B579E41297}"/>
+    <hyperlink ref="L9" r:id="rId2" xr:uid="{5C0C9641-F89C-429D-9BDA-83A8AA52671E}"/>
+    <hyperlink ref="L12" r:id="rId3" xr:uid="{7CA2F957-1200-4DC0-8AE7-7D8B2031492E}"/>
+    <hyperlink ref="L14" r:id="rId4" xr:uid="{546B949B-EACB-4E50-B979-ACF14CB333CA}"/>
+    <hyperlink ref="L16" r:id="rId5" xr:uid="{71BF3B34-237E-4089-A84C-CAAC69B65634}"/>
+    <hyperlink ref="L23" r:id="rId6" xr:uid="{EDE36256-586F-4A20-AAA9-E2DBDEE1B4C7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>